<commit_message>
added lisa's changes and test results
git-svn-id: https://ark-informatics.googlecode.com/svn/ARK/trunk@8225 2beaffb7-5388-1629-0768-26d37724f1fc
</commit_message>
<xml_diff>
--- a/usefulTools/TestFilesAndDocuments/UAT_Registry_Requirements.xlsx
+++ b/usefulTools/TestFilesAndDocuments/UAT_Registry_Requirements.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="168"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32700" windowHeight="20560" tabRatio="168"/>
   </bookViews>
   <sheets>
     <sheet name="UAT Items List" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="208">
   <si>
     <t>Result coding: 1 = Pass (full functionality with no unexpected errors), 0 = Fail (lack of required functionality or reproducible error during testing), 9 = Conditional (partial functionality, error during testing which cannot be reproduced, poor user experience or other constraints) X = Functionality which is desirable for future iterations of the system. these items are not necessary for user acceptance of this version of the system</t>
   </si>
@@ -106,12 +106,6 @@
     <t>1. The user is unable to be located under "Manage Users". 2. The user's access rights for the new substudy are different to their access rights for the WARTN study.</t>
   </si>
   <si>
-    <t>cellis</t>
-  </si>
-  <si>
-    <t>repeated test case. User was not locked out of system</t>
-  </si>
-  <si>
     <t>2.2</t>
   </si>
   <si>
@@ -190,9 +184,6 @@
     <t>1. Study Administrator is unable to modify substudy specific access for users with access to WARTN. 2. The modified user is unable to confirm the appropriate access changes. 3. The user's access to WARTN is affected by substudy access modifications. 4. The user's access to a substudy is governed by WARTN access. 5. Substudy access modifications affect the user's access to WARTN. 6. Substudy access modifications affect  the user's access to other substudies.</t>
   </si>
   <si>
-    <t>on replication of test case, user was not altered</t>
-  </si>
-  <si>
     <t>2.3.2</t>
   </si>
   <si>
@@ -259,24 +250,6 @@
     <t>1. The user is unable to see a list of all studies and substudies. 2. The user is unable to view the study details. 3. The user is unable to modify study details. 4. The user is unable to set the substudy's status to "Archived".</t>
   </si>
   <si>
-    <t>2.4.3</t>
-  </si>
-  <si>
-    <t>A user with "Study Administrator" access to a study and all of its substudies can view a list of all archived substudies in the Study &gt; Study Details tab.</t>
-  </si>
-  <si>
-    <t>1. Log in as a user with "Study Administrator" access to WARTN and all of its substudies. 2. Identify an archived substudy in the Study &gt; Study Details tab. 3. Identify that the study is Archived.</t>
-  </si>
-  <si>
-    <t>1. The user is able to identify archived substudies in the Study &gt; Study Details tab. 2. The user is able to identify if a substudy's status is "Archived". 3. The user is able to identify active studies in the Study &gt; Study Details tab.</t>
-  </si>
-  <si>
-    <t>1. The user is unable to identify archived substudies in the Study &gt; Study Details tab. 2. The user is unable to identify if a substudy's status is "Archived". 3. The user is unable to identify active studies in the Study &gt; Study Details tab.</t>
-  </si>
-  <si>
-    <t>study administrator cannot see archived studies in the list on study details page.</t>
-  </si>
-  <si>
     <t>2.4.4</t>
   </si>
   <si>
@@ -328,30 +301,12 @@
     <t>2.4.7</t>
   </si>
   <si>
-    <t>A user with access to a study and all of its substudies can identify the collections and biospecimens for a patient for all active studies when viewing the Subject &gt; Subject Biospecimen tab from the context of the parent study.</t>
-  </si>
-  <si>
-    <t>1. Log in as a user with access to WARTN and all of its substudies. 2. Under Study &gt; Study Details, enter the context of the WARTN study. 3. Under Subject &gt; Demographic Data, enter the context of a patient with biospecimens associated to multiple active substudies, and an archived substudy. 4. In the Subject &gt; Subject Biospecimen tab, identify the collections associated with active substudies, and the collections associated with archived substudies.</t>
-  </si>
-  <si>
-    <t>1. The user is able to view the Subject &gt; Subject Biospecimen tab from the context of the parent study. 2. The user is able to see all collections, biospecimens, and transactions assigned to active substudies. 3. The user is unable to identify collections, biospecimens, or transactions assigned to archived substudies.</t>
-  </si>
-  <si>
-    <t>1. The user is unable to view the Subject &gt; Subject Biospecimen tab from the context of the parent study. 2. The user is unable to see all collections, biospecimens, and transactions assigned to active substudies. 3. The user is able to identify collections, biospecimens, or transactions assigned to archived substudies.</t>
-  </si>
-  <si>
     <t>Lisa; “  I am happy to accept that you can see a list of substudies the patient has consented to when in the Subject page of the parent study but you have to be in the context of the substudy to see the collections and biospecimens for that substudy.  The vast majority of our patients are only in one study and we have no patients in more than two so its not a big deal practically.  Happy to sign off.”</t>
   </si>
   <si>
     <t>2.4.8</t>
   </si>
   <si>
-    <t>A user with access to a study and all of its substudies can identify the collections and biospecimens for a patient for all active studies when viewing the Subject &gt; Biospecimen tab from the context of the parent study.</t>
-  </si>
-  <si>
-    <t>1. Log in as a user with access to WARTN and all of its substudies. 2. Under Study &gt; Study Details, enter the context of the WARTN study. 3. Under Subject &gt; Demographic Data, enter the context of a patient with biospecimens associated to multiple active substudies, and an archived substudy. 4. In the Subject &gt; Biospecimen tab, identify the collections associated with active substudies, and the collections assosciated with archived substudies.</t>
-  </si>
-  <si>
     <t>1. The user is able to view the Subject &gt; Biospecimen tab from the context of the parent study. 2. The user is able to see all collections, biospecimens, and transactions assigned to active substudies. 3. The user is unable to identify collections, biospecimens, or transactions assigned to archived substudies.</t>
   </si>
   <si>
@@ -619,18 +574,12 @@
     <t>1. The user is able to create a new collection for a subject.</t>
   </si>
   <si>
-    <t>new subject created successfully</t>
-  </si>
-  <si>
     <t>A user with "LIMS Read-Only" access to a study cannot define new collections.</t>
   </si>
   <si>
     <t>1. The user is unable to create a new subject.</t>
   </si>
   <si>
-    <t>unable to create new subjects</t>
-  </si>
-  <si>
     <t>sequential collection numbering across all studies and substudies (C-01234)</t>
   </si>
   <si>
@@ -649,13 +598,52 @@
     <t>USER EXPERIENCE: When a collection is in context, the study or substudy that the collection is associated with should be readily visible.</t>
   </si>
   <si>
-    <t>USER EXPERIENCE: When a collection is in context, the collection ID should always be visible, with the consent status for the assosciated substudy.</t>
-  </si>
-  <si>
     <t>SECURITY &amp; BACKUP</t>
   </si>
   <si>
-    <t>Users of all access levels should only be able to see the studies and substudies they have access to.</t>
+    <t>Users of all access levels should only be able to see the studies and substudies they have access to.  Note that a parent study permission is passed down to substudies</t>
+  </si>
+  <si>
+    <t>in discussion</t>
+  </si>
+  <si>
+    <t>A user with access to a substudy  can identify the collections and biospecimens for a patient for only that substudy in context  when viewing the Subject &gt; Subject Biospecimen tab from the context of the substudy.</t>
+  </si>
+  <si>
+    <t>1. The user is able to view the Subject &gt; Subject Biospecimen tab from the context of the child study. 2. The user is able to see all collections, biospecimens, and transactions assigned to the substudy. 3. The user is unable to identify collections, biospecimens, or transactions assigned to archived substudies.</t>
+  </si>
+  <si>
+    <t>1. The user is unable to view the Subject &gt; Subject Biospecimen tab from the context of the sub study. 2. The user is unable to see all collections, biospecimens, and transactions assigned to active substudies. 3. The user is able to identify collections, biospecimens, or transactions assigned to archived substudies.</t>
+  </si>
+  <si>
+    <t>A user with access to a substudy can identify the collections and biospecimens for a patient for the substudies when viewing the Subject &gt; Biospecimen tab from the context of the substudy.</t>
+  </si>
+  <si>
+    <t>1. Log in as a user with access to WARTN and all of its substudies. 2. Under Study &gt; Study Details, enter the context of the WARTN substudy. 3. Under Subject &gt; Demographic Data, enter the context of a patient with biospecimens associated to multiple active substudies, and an archived substudy. 4. In the Subject &gt; Biospecimen tab, identify the collections associated with active substudies, and the collections assosciated with archived substudies.</t>
+  </si>
+  <si>
+    <t>1. Log in as a user with access to WARTN and all of its substudies. 2. Under Study &gt; Study Details, enter the context of the WARTN substudy. 3. Under Subject &gt; Demographic Data, enter the context of a patient with biospecimens associated to multiple active substudies, and an archived substudy. 4. In the Subject &gt; Biospecimen tab, identify the biospecimens associated with active substudies, and thebiospecimens assosciated with archived substudies.</t>
+  </si>
+  <si>
+    <t>LISA</t>
+  </si>
+  <si>
+    <t>Lisaq</t>
+  </si>
+  <si>
+    <t>8/7/2013 12.05</t>
+  </si>
+  <si>
+    <t>new collection created successfully</t>
+  </si>
+  <si>
+    <t>unable to create new collections</t>
+  </si>
+  <si>
+    <t>in discussion, propsed change</t>
+  </si>
+  <si>
+    <t>ARK-1042</t>
   </si>
 </sst>
 </file>
@@ -667,7 +655,7 @@
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yy\ hh:mm"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -750,6 +738,22 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -813,10 +817,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -971,8 +979,21 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1372,21 +1393,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView tabSelected="1" zoomScale="123" zoomScaleNormal="123" zoomScalePageLayoutView="123" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="32" style="3" customWidth="1"/>
-    <col min="3" max="3" width="46.33203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="51.33203125" style="4" customWidth="1"/>
     <col min="4" max="4" width="33.5" style="4" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="5"/>
-    <col min="7" max="7" width="19.83203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="37.6640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="8" style="5" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" style="5" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" style="6"/>
-    <col min="9" max="9" width="10.83203125" style="7"/>
+    <col min="9" max="9" width="15" style="7" customWidth="1"/>
     <col min="13" max="1020" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
@@ -1404,7 +1425,7 @@
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
     </row>
-    <row r="3" spans="1:13" ht="16.5" customHeight="1">
+    <row r="3" spans="1:13" ht="16.5" customHeight="1" thickBot="1">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
@@ -1433,7 +1454,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="36" customHeight="1">
+    <row r="4" spans="1:13" ht="36" customHeight="1" thickTop="1" thickBot="1">
       <c r="A4" s="15"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
@@ -1441,14 +1462,14 @@
       <c r="E4" s="17"/>
       <c r="F4" s="18"/>
       <c r="G4" s="18"/>
-      <c r="H4" s="19"/>
+      <c r="H4" s="18"/>
       <c r="I4" s="20"/>
       <c r="J4" s="21"/>
       <c r="K4" s="21"/>
       <c r="L4" s="21"/>
       <c r="M4" s="21"/>
     </row>
-    <row r="5" spans="1:13" ht="15.75" customHeight="1">
+    <row r="5" spans="1:13" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -1492,8 +1513,12 @@
       <c r="E7" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="27"/>
+      <c r="F7" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="27">
+        <v>41493.496527777781</v>
+      </c>
       <c r="H7" s="19">
         <v>1</v>
       </c>
@@ -1515,14 +1540,18 @@
       <c r="E8" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="27"/>
+      <c r="F8" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="27">
+        <v>41493.478472222225</v>
+      </c>
       <c r="H8" s="19">
         <v>1</v>
       </c>
       <c r="I8" s="28"/>
     </row>
-    <row r="9" spans="1:13" ht="124.5" customHeight="1">
+    <row r="9" spans="1:13" ht="131" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
@@ -1539,24 +1568,22 @@
         <v>27</v>
       </c>
       <c r="F9" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="27">
+        <v>41493.498611111114</v>
+      </c>
+      <c r="H9" s="30">
+        <v>1</v>
+      </c>
+      <c r="I9" s="28"/>
+    </row>
+    <row r="10" spans="1:13" ht="24" customHeight="1">
+      <c r="A10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="27">
-        <v>41337.635416666701</v>
-      </c>
-      <c r="H9" s="30">
-        <v>1</v>
-      </c>
-      <c r="I9" s="28" t="s">
+      <c r="B10" s="22" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="15" customHeight="1">
-      <c r="A10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>31</v>
       </c>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
@@ -1566,25 +1593,25 @@
     </row>
     <row r="11" spans="1:13" ht="69" customHeight="1" thickTop="1" thickBot="1">
       <c r="A11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="E11" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>35</v>
-      </c>
       <c r="F11" s="26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G11" s="27">
-        <v>41262.555555555598</v>
+        <v>41493.458333333336</v>
       </c>
       <c r="H11" s="30">
         <v>1</v>
@@ -1593,25 +1620,25 @@
     </row>
     <row r="12" spans="1:13" ht="83.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="E12" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>40</v>
-      </c>
       <c r="F12" s="26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G12" s="27">
-        <v>41262.555555555598</v>
+        <v>41493.465277777781</v>
       </c>
       <c r="H12" s="30">
         <v>1</v>
@@ -1620,25 +1647,25 @@
     </row>
     <row r="13" spans="1:13" ht="83.25" customHeight="1">
       <c r="A13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="E13" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>44</v>
-      </c>
       <c r="F13" s="26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G13" s="27">
-        <v>41262.555555555598</v>
+        <v>41493.466666666667</v>
       </c>
       <c r="H13" s="30">
         <v>1</v>
@@ -1647,25 +1674,25 @@
     </row>
     <row r="14" spans="1:13" ht="83.25" customHeight="1">
       <c r="A14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="E14" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>48</v>
-      </c>
       <c r="F14" s="26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G14" s="27">
-        <v>41262.554166666698</v>
+        <v>41493.467361111114</v>
       </c>
       <c r="H14" s="30">
         <v>1</v>
@@ -1674,10 +1701,10 @@
     </row>
     <row r="15" spans="1:13" ht="15" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
@@ -1685,53 +1712,57 @@
       <c r="F15" s="23"/>
       <c r="G15" s="23"/>
     </row>
-    <row r="16" spans="1:13" ht="150.75" customHeight="1">
+    <row r="16" spans="1:13" ht="187" customHeight="1">
       <c r="A16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="D16" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="E16" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="25" t="s">
-        <v>55</v>
-      </c>
       <c r="F16" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" s="27">
-        <v>41337.638194444502</v>
+        <v>34</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>206</v>
       </c>
       <c r="H16" s="30">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I16" s="28" t="s">
-        <v>56</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="150.75" customHeight="1">
       <c r="A17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="E17" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="27"/>
+      <c r="F17" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="27">
+        <v>41493.479166666664</v>
+      </c>
       <c r="H17" s="30">
         <v>1</v>
       </c>
@@ -1739,39 +1770,37 @@
     </row>
     <row r="18" spans="1:10" ht="206.25" customHeight="1">
       <c r="A18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="E18" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" s="25" t="s">
-        <v>66</v>
-      </c>
       <c r="F18" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" s="27">
-        <v>41337.638194444502</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="G18" s="27"/>
       <c r="H18" s="30">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I18" s="28" t="s">
-        <v>56</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
@@ -1781,480 +1810,486 @@
     </row>
     <row r="20" spans="1:10" ht="90.75" customHeight="1">
       <c r="A20" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="E20" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="F20" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="27">
+        <v>41493.534722222219</v>
+      </c>
+      <c r="H20" s="30">
+        <v>1</v>
+      </c>
+      <c r="I20" s="28"/>
+    </row>
+    <row r="21" spans="1:10" ht="83.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A21" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="B21" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="E20" s="25" t="s">
+      <c r="C21" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="F20" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="G20" s="27">
-        <v>41262.579166666699</v>
-      </c>
-      <c r="H20" s="30">
-        <v>1</v>
-      </c>
-      <c r="I20" s="28"/>
-    </row>
-    <row r="21" spans="1:10" ht="83.25" customHeight="1">
-      <c r="A21" s="2" t="s">
+      <c r="D21" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="E21" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="F21" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="27">
+        <v>41493.484722222223</v>
+      </c>
+      <c r="H21" s="30">
+        <v>1</v>
+      </c>
+      <c r="I21" s="28"/>
+    </row>
+    <row r="22" spans="1:10" ht="73.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A22" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="B22" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="25" t="s">
+      <c r="C22" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="F21" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="G21" s="27">
-        <v>41262.586805555598</v>
-      </c>
-      <c r="H21" s="30">
-        <v>1</v>
-      </c>
-      <c r="I21" s="28"/>
-    </row>
-    <row r="22" spans="1:10" ht="85.5" customHeight="1">
-      <c r="A22" s="2" t="s">
+      <c r="D22" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="E22" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="F22" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="27">
+        <v>41493.536111111112</v>
+      </c>
+      <c r="H22" s="30">
+        <v>1</v>
+      </c>
+      <c r="I22" s="28"/>
+    </row>
+    <row r="23" spans="1:10" ht="132" customHeight="1">
+      <c r="A23" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="B23" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="C23" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="F22" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G22" s="27">
-        <v>41262.564583217601</v>
-      </c>
-      <c r="H22" s="31">
-        <v>1</v>
-      </c>
-      <c r="I22" s="28" t="s">
+      <c r="D23" s="25" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="73.5" customHeight="1">
-      <c r="A23" s="2" t="s">
+      <c r="E23" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="F23" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" s="27">
+        <v>41493.486111111109</v>
+      </c>
+      <c r="H23" s="30">
+        <v>1</v>
+      </c>
+      <c r="I23" s="28"/>
+    </row>
+    <row r="24" spans="1:10" ht="113" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A24" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="B24" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="D23" s="24" t="s">
+      <c r="C24" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="D24" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="F23" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="G23" s="27">
-        <v>41262.581250000003</v>
-      </c>
-      <c r="H23" s="30">
-        <v>1</v>
-      </c>
-      <c r="I23" s="28"/>
-    </row>
-    <row r="24" spans="1:10" ht="98.25" customHeight="1">
-      <c r="A24" s="2" t="s">
+      <c r="E24" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="F24" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" s="27">
+        <v>41493.496527777781</v>
+      </c>
+      <c r="H24" s="30">
+        <v>1</v>
+      </c>
+      <c r="I24" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="C24" s="25" t="s">
+    </row>
+    <row r="25" spans="1:10" ht="171.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A25" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D24" s="25" t="s">
+      <c r="B25" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25" s="27">
+        <v>41493</v>
+      </c>
+      <c r="H25" s="31">
+        <v>1</v>
+      </c>
+      <c r="I25" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="E24" s="25" t="s">
+    </row>
+    <row r="26" spans="1:10" ht="171.25" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A26" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F24" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="G24" s="27">
-        <v>41262.581944328696</v>
-      </c>
-      <c r="H24" s="30">
-        <v>1</v>
-      </c>
-      <c r="I24" s="28"/>
-    </row>
-    <row r="25" spans="1:10" ht="113" customHeight="1">
-      <c r="A25" s="2" t="s">
+      <c r="B26" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="D26" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="E26" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="F26" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="H26" s="31">
+        <v>1</v>
+      </c>
+      <c r="I26" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="J26" t="s">
         <v>97</v>
       </c>
-      <c r="D25" s="25" t="s">
+    </row>
+    <row r="27" spans="1:10" ht="153" customHeight="1">
+      <c r="A27" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E25" s="25" t="s">
+      <c r="B27" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="F25" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G25" s="27">
-        <v>41262.564583217601</v>
-      </c>
-      <c r="H25" s="30">
-        <v>1</v>
-      </c>
-      <c r="I25" s="28" t="s">
+      <c r="C27" s="24" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="171.25" customHeight="1">
-      <c r="A26" s="2" t="s">
+      <c r="D27" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="E27" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="F27" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27" s="27">
+        <v>41493</v>
+      </c>
+      <c r="H27" s="30">
+        <v>1</v>
+      </c>
+      <c r="I27" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="D26" s="24" t="s">
+    </row>
+    <row r="28" spans="1:10" ht="109.5" customHeight="1">
+      <c r="A28" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E26" s="24" t="s">
+      <c r="B28" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="F26" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="G26" s="27">
-        <v>41262.595833217601</v>
-      </c>
-      <c r="H26" s="31">
-        <v>1</v>
-      </c>
-      <c r="I26" s="28" t="s">
+      <c r="C28" s="25" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="171.25" customHeight="1">
-      <c r="A27" s="2" t="s">
+      <c r="D28" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="E28" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="F28" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G28" s="27">
+        <v>41493</v>
+      </c>
+      <c r="H28" s="30">
+        <v>1</v>
+      </c>
+      <c r="I28" s="28"/>
+    </row>
+    <row r="29" spans="1:10" ht="128" customHeight="1">
+      <c r="A29" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="24" t="s">
+      <c r="B29" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="E27" s="24" t="s">
+      <c r="C29" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="F27" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="G27" s="27">
-        <v>41262.601388888899</v>
-      </c>
-      <c r="H27" s="31">
-        <v>1</v>
-      </c>
-      <c r="I27" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="J27" t="s">
+      <c r="D29" s="25" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="153" customHeight="1">
-      <c r="A28" s="2" t="s">
+      <c r="E29" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="F29" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G29" s="27">
+        <v>406735.02083333331</v>
+      </c>
+      <c r="H29" s="30">
+        <v>1</v>
+      </c>
+      <c r="I29" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="C28" s="24" t="s">
+    </row>
+    <row r="30" spans="1:10" ht="109.5" customHeight="1">
+      <c r="A30" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D28" s="24" t="s">
+      <c r="B30" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="E28" s="24" t="s">
+      <c r="C30" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="F28" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G28" s="27">
-        <v>41337.657638888901</v>
-      </c>
-      <c r="H28" s="30">
-        <v>1</v>
-      </c>
-      <c r="I28" s="28" t="s">
+      <c r="D30" s="25" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="109.5" customHeight="1">
-      <c r="A29" s="2" t="s">
+      <c r="E30" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="B29" s="25" t="s">
+      <c r="F30" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="G30" s="27">
+        <v>41493.022916666669</v>
+      </c>
+      <c r="H30" s="31">
+        <v>1</v>
+      </c>
+      <c r="I30" s="28"/>
+    </row>
+    <row r="31" spans="1:10" ht="93.75" customHeight="1">
+      <c r="A31" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="B31" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D29" s="25" t="s">
+      <c r="C31" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="E29" s="25" t="s">
+      <c r="D31" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="F29" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="G29" s="27">
-        <v>41337.6020832176</v>
-      </c>
-      <c r="H29" s="30">
-        <v>1</v>
-      </c>
-      <c r="I29" s="28"/>
-    </row>
-    <row r="30" spans="1:10" ht="124.5" customHeight="1">
-      <c r="A30" s="2" t="s">
+      <c r="E31" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="B30" s="25" t="s">
+      <c r="F31" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="G31" s="27">
+        <v>41493.024305555555</v>
+      </c>
+      <c r="H31" s="31">
+        <v>1</v>
+      </c>
+      <c r="I31" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="C30" s="25" t="s">
+    </row>
+    <row r="32" spans="1:10" ht="109.5" customHeight="1">
+      <c r="A32" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D30" s="25" t="s">
+      <c r="B32" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="E30" s="25" t="s">
+      <c r="C32" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="F30" s="26"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="30">
-        <v>1</v>
-      </c>
-      <c r="I30" s="28" t="s">
+      <c r="D32" s="25" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="109.5" customHeight="1">
-      <c r="A31" s="2" t="s">
+      <c r="E32" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="B31" s="25" t="s">
+      <c r="F32" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G32" s="27">
+        <v>41493.025694444441</v>
+      </c>
+      <c r="H32" s="30">
+        <v>1</v>
+      </c>
+      <c r="I32" s="28"/>
+    </row>
+    <row r="33" spans="1:13" ht="124.5" customHeight="1">
+      <c r="A33" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="B33" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="D31" s="25" t="s">
+      <c r="C33" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="E31" s="25" t="s">
+      <c r="D33" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="F31" s="26"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="31">
-        <v>1</v>
-      </c>
-      <c r="I31" s="28"/>
-    </row>
-    <row r="32" spans="1:10" ht="93.75" customHeight="1">
-      <c r="A32" s="2" t="s">
+      <c r="E33" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="B32" s="25" t="s">
+      <c r="F33" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G33" s="27">
+        <v>41493.026388888888</v>
+      </c>
+      <c r="H33" s="30">
+        <v>1</v>
+      </c>
+      <c r="I33" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="C32" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="D32" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="E32" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="F32" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G32" s="27">
-        <v>40973.6645832176</v>
-      </c>
-      <c r="H32" s="31">
-        <v>1</v>
-      </c>
-      <c r="I32" s="28" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="109.5" customHeight="1">
-      <c r="A33" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B33" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="C33" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="D33" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="E33" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="F33" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="G33" s="27">
-        <v>41262.604860995401</v>
-      </c>
-      <c r="H33" s="30">
-        <v>1</v>
-      </c>
-      <c r="I33" s="28"/>
     </row>
     <row r="34" spans="1:13" ht="124.5" customHeight="1">
       <c r="A34" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="E34" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="F34" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G34" s="27">
+        <v>41493.527083333334</v>
+      </c>
+      <c r="H34" s="30">
+        <v>1</v>
+      </c>
+      <c r="I34" s="28"/>
+    </row>
+    <row r="35" spans="1:13" ht="15" customHeight="1">
+      <c r="A35" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B35" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+    </row>
+    <row r="36" spans="1:13" ht="100" customHeight="1">
+      <c r="A36" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B36" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D36" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="B34" s="25" t="s">
+      <c r="E36" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C34" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="D34" s="25" t="s">
-        <v>149</v>
-      </c>
-      <c r="E34" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="F34" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="G34" s="27">
-        <v>41262.605555555601</v>
-      </c>
-      <c r="H34" s="30">
-        <v>1</v>
-      </c>
-      <c r="I34" s="28" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="124.5" customHeight="1">
-      <c r="A35" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B35" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="C35" s="25" t="s">
-        <v>153</v>
-      </c>
-      <c r="D35" s="25" t="s">
-        <v>154</v>
-      </c>
-      <c r="E35" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="F35" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="G35" s="27">
-        <v>41262.613888888904</v>
-      </c>
-      <c r="H35" s="30">
-        <v>1</v>
-      </c>
-      <c r="I35" s="28"/>
-    </row>
-    <row r="36" spans="1:13" ht="15" customHeight="1">
-      <c r="A36" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B36" s="22" t="s">
-        <v>157</v>
-      </c>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
+      <c r="F36" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G36" s="27">
+        <v>41493.527083333334</v>
+      </c>
+      <c r="H36" s="30">
+        <v>1</v>
+      </c>
+      <c r="I36" s="28"/>
     </row>
     <row r="37" spans="1:13" ht="100" customHeight="1">
       <c r="A37" s="2" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="B37" s="24" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="E37" s="25" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="F37" s="26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G37" s="27">
-        <v>41262.615972106498</v>
+        <v>41493.527083333334</v>
       </c>
       <c r="H37" s="30">
         <v>1</v>
@@ -2263,25 +2298,25 @@
     </row>
     <row r="38" spans="1:13" ht="100" customHeight="1">
       <c r="A38" s="2" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="B38" s="24" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="E38" s="25" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="F38" s="26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G38" s="27">
-        <v>41262.615972106498</v>
+        <v>41493.527083333334</v>
       </c>
       <c r="H38" s="30">
         <v>1</v>
@@ -2290,25 +2325,25 @@
     </row>
     <row r="39" spans="1:13" ht="100" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="E39" s="25" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="F39" s="26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G39" s="27">
-        <v>41262.616666666698</v>
+        <v>41493.527083333334</v>
       </c>
       <c r="H39" s="30">
         <v>1</v>
@@ -2317,25 +2352,25 @@
     </row>
     <row r="40" spans="1:13" ht="100" customHeight="1">
       <c r="A40" s="2" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="B40" s="24" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="E40" s="25" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="F40" s="26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G40" s="27">
-        <v>41262.616666666698</v>
+        <v>41493.527083333334</v>
       </c>
       <c r="H40" s="30">
         <v>1</v>
@@ -2344,507 +2379,505 @@
     </row>
     <row r="41" spans="1:13" ht="100" customHeight="1">
       <c r="A41" s="2" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="B41" s="24" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="C41" s="25" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="E41" s="25" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="F41" s="26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G41" s="27">
-        <v>41262.618055555598</v>
+        <v>41493.527083333334</v>
       </c>
       <c r="H41" s="30">
         <v>1</v>
       </c>
-      <c r="I41" s="28"/>
+      <c r="I41" s="28" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="42" spans="1:13" ht="100" customHeight="1">
       <c r="A42" s="2" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="C42" s="25" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="D42" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="E42" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="F42" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G42" s="27">
+        <v>41493.527083333334</v>
+      </c>
+      <c r="H42" s="30">
+        <v>1</v>
+      </c>
+      <c r="I42" s="28"/>
+    </row>
+    <row r="43" spans="1:13" ht="36" customHeight="1">
+      <c r="A43" s="15"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="34"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="21"/>
+      <c r="K43" s="21"/>
+      <c r="L43" s="21"/>
+      <c r="M43" s="21"/>
+    </row>
+    <row r="44" spans="1:13" ht="15.75" customHeight="1">
+      <c r="B44" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="E42" s="25" t="s">
-        <v>162</v>
-      </c>
-      <c r="F42" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="G42" s="27">
-        <v>41337.677083217597</v>
-      </c>
-      <c r="H42" s="30">
-        <v>1</v>
-      </c>
-      <c r="I42" s="28" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" ht="100" customHeight="1">
-      <c r="A43" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B43" s="24" t="s">
-        <v>175</v>
-      </c>
-      <c r="C43" s="25" t="s">
-        <v>160</v>
-      </c>
-      <c r="D43" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="E43" s="25" t="s">
-        <v>162</v>
-      </c>
-      <c r="F43" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="G43" s="27">
-        <v>41262.619444328702</v>
-      </c>
-      <c r="H43" s="30">
-        <v>1</v>
-      </c>
-      <c r="I43" s="28"/>
-    </row>
-    <row r="44" spans="1:13" ht="36" customHeight="1">
-      <c r="A44" s="15"/>
-      <c r="B44" s="16"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="33"/>
-      <c r="G44" s="33"/>
-      <c r="H44" s="34"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="21"/>
-      <c r="K44" s="21"/>
-      <c r="L44" s="21"/>
-      <c r="M44" s="21"/>
-    </row>
-    <row r="45" spans="1:13" ht="15.75" customHeight="1">
-      <c r="B45" s="22" t="s">
-        <v>176</v>
-      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="35"/>
+    </row>
+    <row r="45" spans="1:13" ht="15" customHeight="1">
+      <c r="B45" s="22"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="35"/>
       <c r="G45" s="35"/>
     </row>
-    <row r="46" spans="1:13" ht="15" customHeight="1">
-      <c r="B46" s="22"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="35"/>
-    </row>
-    <row r="47" spans="1:13" ht="75.75" customHeight="1">
+    <row r="46" spans="1:13" ht="112">
+      <c r="B46" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="C46" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="D46" s="36"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G46" s="52">
+        <v>41493.527777777781</v>
+      </c>
+      <c r="H46" s="19">
+        <v>1</v>
+      </c>
+      <c r="I46" s="28"/>
+    </row>
+    <row r="47" spans="1:13" ht="84">
       <c r="B47" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="C47" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="D47" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="E47" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="F47" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G47" s="53">
+        <v>41493.534722222219</v>
+      </c>
+      <c r="H47" s="19">
+        <v>1</v>
+      </c>
+      <c r="I47" s="28"/>
+    </row>
+    <row r="48" spans="1:13" ht="98">
+      <c r="B48" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="C48" s="36" t="s">
+        <v>168</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="F48" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G48" s="52">
+        <v>41493.536111111112</v>
+      </c>
+      <c r="H48" s="37">
+        <v>1</v>
+      </c>
+      <c r="I48" s="28" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1024" s="44" customFormat="1" ht="42">
+      <c r="A49" s="38"/>
+      <c r="B49" s="39" t="s">
+        <v>171</v>
+      </c>
+      <c r="C49" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="D49" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="E49" s="40" t="s">
+        <v>174</v>
+      </c>
+      <c r="F49" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G49" s="54">
+        <v>41493.537499999999</v>
+      </c>
+      <c r="H49" s="42">
+        <v>1</v>
+      </c>
+      <c r="I49" s="43"/>
+      <c r="AMG49"/>
+      <c r="AMH49"/>
+      <c r="AMI49"/>
+      <c r="AMJ49"/>
+    </row>
+    <row r="50" spans="1:1024" ht="36" customHeight="1">
+      <c r="A50" s="15"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="33"/>
+      <c r="H50" s="34"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="21"/>
+      <c r="K50" s="21"/>
+      <c r="L50" s="21"/>
+      <c r="M50" s="21"/>
+    </row>
+    <row r="51" spans="1:1024" ht="15.75" customHeight="1">
+      <c r="B51" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="F51" s="35"/>
+      <c r="G51" s="35"/>
+    </row>
+    <row r="52" spans="1:1024" ht="15" customHeight="1">
+      <c r="B52" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="F52" s="23"/>
+      <c r="G52" s="23"/>
+    </row>
+    <row r="53" spans="1:1024" ht="61.5" customHeight="1">
+      <c r="B53" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="C47" s="25" t="s">
+      <c r="C53" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="D53" s="25"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G53" s="45">
+        <v>41493.53125</v>
+      </c>
+      <c r="H53" s="19">
+        <v>1</v>
+      </c>
+      <c r="I53" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="D47" s="36"/>
-      <c r="E47" s="36"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="19">
-        <v>1</v>
-      </c>
-      <c r="I47" s="28"/>
-    </row>
-    <row r="48" spans="1:13" ht="70.5" customHeight="1">
-      <c r="B48" s="24" t="s">
+    </row>
+    <row r="54" spans="1:1024" ht="36" customHeight="1">
+      <c r="A54" s="15"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="33"/>
+      <c r="G54" s="33"/>
+      <c r="H54" s="34"/>
+      <c r="I54" s="20"/>
+      <c r="J54" s="21"/>
+      <c r="K54" s="21"/>
+      <c r="L54" s="21"/>
+      <c r="M54" s="21"/>
+    </row>
+    <row r="55" spans="1:1024" ht="15.75" customHeight="1">
+      <c r="B55" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="C48" s="25" t="s">
-        <v>180</v>
-      </c>
-      <c r="D48" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="E48" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="F48" s="26"/>
-      <c r="G48" s="26"/>
-      <c r="H48" s="19">
-        <v>1</v>
-      </c>
-      <c r="I48" s="28"/>
-    </row>
-    <row r="49" spans="1:1024" ht="60" customHeight="1">
-      <c r="B49" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="C49" s="36" t="s">
-        <v>183</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="F49" s="26"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="37">
-        <v>1</v>
-      </c>
-      <c r="I49" s="28" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1024" s="44" customFormat="1" ht="45.75" customHeight="1">
-      <c r="A50" s="38"/>
-      <c r="B50" s="39" t="s">
-        <v>186</v>
-      </c>
-      <c r="C50" s="40" t="s">
-        <v>187</v>
-      </c>
-      <c r="D50" s="40" t="s">
-        <v>188</v>
-      </c>
-      <c r="E50" s="40" t="s">
-        <v>189</v>
-      </c>
-      <c r="F50" s="41"/>
-      <c r="G50" s="41"/>
-      <c r="H50" s="42">
-        <v>1</v>
-      </c>
-      <c r="I50" s="43"/>
-      <c r="AMG50"/>
-      <c r="AMH50"/>
-      <c r="AMI50"/>
-      <c r="AMJ50"/>
-    </row>
-    <row r="51" spans="1:1024" ht="36" customHeight="1">
-      <c r="A51" s="15"/>
-      <c r="B51" s="16"/>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="33"/>
-      <c r="G51" s="33"/>
-      <c r="H51" s="34"/>
-      <c r="I51" s="20"/>
-      <c r="J51" s="21"/>
-      <c r="K51" s="21"/>
-      <c r="L51" s="21"/>
-      <c r="M51" s="21"/>
-    </row>
-    <row r="52" spans="1:1024" ht="15.75" customHeight="1">
-      <c r="B52" s="22" t="s">
-        <v>190</v>
-      </c>
-      <c r="F52" s="35"/>
-      <c r="G52" s="35"/>
-    </row>
-    <row r="53" spans="1:1024" ht="15" customHeight="1">
-      <c r="B53" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="F53" s="23"/>
-      <c r="G53" s="23"/>
-    </row>
-    <row r="54" spans="1:1024" ht="61.5" customHeight="1">
-      <c r="B54" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="C54" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G54" s="45">
-        <v>41338.534722106502</v>
-      </c>
-      <c r="H54" s="19">
-        <v>1</v>
-      </c>
-      <c r="I54" s="28" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1024" ht="36" customHeight="1">
-      <c r="A55" s="15"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="33"/>
-      <c r="G55" s="33"/>
-      <c r="H55" s="34"/>
-      <c r="I55" s="20"/>
-      <c r="J55" s="21"/>
-      <c r="K55" s="21"/>
-      <c r="L55" s="21"/>
-      <c r="M55" s="21"/>
+      <c r="F55" s="35"/>
+      <c r="G55" s="35"/>
     </row>
     <row r="56" spans="1:1024" ht="15.75" customHeight="1">
-      <c r="B56" s="22" t="s">
-        <v>194</v>
-      </c>
+      <c r="B56" s="22"/>
       <c r="F56" s="35"/>
       <c r="G56" s="35"/>
     </row>
-    <row r="57" spans="1:1024" ht="15.75" customHeight="1">
-      <c r="B57" s="22"/>
+    <row r="57" spans="1:1024" ht="15" customHeight="1">
+      <c r="B57" s="22" t="s">
+        <v>180</v>
+      </c>
       <c r="F57" s="35"/>
       <c r="G57" s="35"/>
     </row>
-    <row r="58" spans="1:1024" ht="15" customHeight="1">
-      <c r="B58" s="22" t="s">
-        <v>195</v>
-      </c>
-      <c r="F58" s="35"/>
-      <c r="G58" s="35"/>
-    </row>
-    <row r="59" spans="1:1024" ht="73.5" customHeight="1">
+    <row r="58" spans="1:1024" ht="73.5" customHeight="1">
+      <c r="B58" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="C58" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="D58" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="E58" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="F58" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G58" s="45">
+        <v>41493.541666666664</v>
+      </c>
+      <c r="H58" s="19">
+        <v>1</v>
+      </c>
+      <c r="I58" s="28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1024" ht="72" customHeight="1">
       <c r="B59" s="24" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="C59" s="25" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="D59" s="25" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="E59" s="25" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="F59" s="26" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="G59" s="45">
-        <v>41338.534722106502</v>
+        <v>41493.545138888891</v>
       </c>
       <c r="H59" s="19">
         <v>1</v>
       </c>
       <c r="I59" s="28" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1024" ht="72" customHeight="1">
-      <c r="B60" s="24" t="s">
-        <v>200</v>
-      </c>
-      <c r="C60" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="D60" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="E60" s="25" t="s">
-        <v>201</v>
-      </c>
-      <c r="F60" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G60" s="45">
-        <v>41338.534722106502</v>
-      </c>
-      <c r="H60" s="19">
-        <v>1</v>
-      </c>
-      <c r="I60" s="28" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1024" ht="15" customHeight="1">
-      <c r="B61" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="F61" s="35"/>
-      <c r="G61" s="35"/>
-    </row>
-    <row r="62" spans="1:1024" ht="105" customHeight="1">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1024" ht="15" customHeight="1">
+      <c r="B60" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="F60" s="35"/>
+      <c r="G60" s="35"/>
+    </row>
+    <row r="61" spans="1:1024" ht="105" customHeight="1">
+      <c r="B61" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="C61" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="D61" s="25"/>
+      <c r="E61" s="25"/>
+      <c r="F61" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G61" s="52">
+        <v>41493.490277777775</v>
+      </c>
+      <c r="H61" s="19">
+        <v>1</v>
+      </c>
+      <c r="I61" s="28"/>
+    </row>
+    <row r="62" spans="1:1024" ht="69.75" customHeight="1">
       <c r="B62" s="24" t="s">
-        <v>203</v>
-      </c>
-      <c r="C62" s="25" t="s">
-        <v>204</v>
-      </c>
-      <c r="D62" s="25"/>
-      <c r="E62" s="25"/>
-      <c r="F62" s="26"/>
-      <c r="G62" s="26"/>
+        <v>188</v>
+      </c>
+      <c r="C62" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="F62" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G62" s="52">
+        <v>41493.490277777775</v>
+      </c>
       <c r="H62" s="19">
         <v>1</v>
       </c>
       <c r="I62" s="28"/>
     </row>
-    <row r="63" spans="1:1024" ht="69.75" customHeight="1">
-      <c r="B63" s="24" t="s">
-        <v>205</v>
-      </c>
-      <c r="C63" s="24" t="s">
-        <v>205</v>
-      </c>
-      <c r="F63" s="26"/>
-      <c r="G63" s="26"/>
-      <c r="H63" s="19">
-        <v>1</v>
-      </c>
-      <c r="I63" s="28"/>
-    </row>
-    <row r="64" spans="1:1024" s="44" customFormat="1" ht="49.5" customHeight="1">
+    <row r="63" spans="1:1024" s="44" customFormat="1" ht="56">
+      <c r="A63" s="38"/>
+      <c r="B63" s="46" t="s">
+        <v>189</v>
+      </c>
+      <c r="C63" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="D63" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="E63" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="F63" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="G63" s="54">
+        <v>41493.490972222222</v>
+      </c>
+      <c r="H63" s="42">
+        <v>1</v>
+      </c>
+      <c r="I63" s="43" t="s">
+        <v>190</v>
+      </c>
+      <c r="AMG63"/>
+      <c r="AMH63"/>
+      <c r="AMI63"/>
+      <c r="AMJ63"/>
+    </row>
+    <row r="64" spans="1:1024" s="44" customFormat="1" ht="56">
       <c r="A64" s="38"/>
       <c r="B64" s="46" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="C64" s="40" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="D64" s="25" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="E64" s="25" t="s">
-        <v>189</v>
-      </c>
-      <c r="F64" s="41"/>
-      <c r="G64" s="41"/>
+        <v>174</v>
+      </c>
+      <c r="F64" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="G64" s="54">
+        <v>41493.490972222222</v>
+      </c>
       <c r="H64" s="42">
         <v>1</v>
       </c>
-      <c r="I64" s="43" t="s">
-        <v>207</v>
-      </c>
+      <c r="I64" s="43"/>
       <c r="AMG64"/>
       <c r="AMH64"/>
       <c r="AMI64"/>
       <c r="AMJ64"/>
     </row>
-    <row r="65" spans="1:1024" s="44" customFormat="1" ht="64.5" customHeight="1">
+    <row r="65" spans="1:1024" s="44" customFormat="1" ht="60" customHeight="1">
       <c r="A65" s="38"/>
-      <c r="B65" s="46" t="s">
-        <v>208</v>
-      </c>
-      <c r="C65" s="40" t="s">
-        <v>187</v>
-      </c>
-      <c r="D65" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="E65" s="25" t="s">
-        <v>189</v>
-      </c>
+      <c r="B65" s="46"/>
+      <c r="C65" s="40"/>
+      <c r="D65" s="25"/>
+      <c r="E65" s="25"/>
       <c r="F65" s="41"/>
       <c r="G65" s="41"/>
-      <c r="H65" s="42">
-        <v>1</v>
-      </c>
+      <c r="H65" s="42"/>
       <c r="I65" s="43"/>
       <c r="AMG65"/>
       <c r="AMH65"/>
       <c r="AMI65"/>
       <c r="AMJ65"/>
     </row>
-    <row r="66" spans="1:1024" s="44" customFormat="1" ht="60" customHeight="1">
-      <c r="A66" s="38"/>
-      <c r="B66" s="46" t="s">
-        <v>209</v>
-      </c>
-      <c r="C66" s="40" t="s">
-        <v>187</v>
-      </c>
-      <c r="D66" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="E66" s="25" t="s">
-        <v>189</v>
-      </c>
-      <c r="F66" s="41"/>
-      <c r="G66" s="41"/>
-      <c r="H66" s="42">
-        <v>1</v>
-      </c>
-      <c r="I66" s="43"/>
-      <c r="AMG66"/>
-      <c r="AMH66"/>
-      <c r="AMI66"/>
-      <c r="AMJ66"/>
-    </row>
-    <row r="67" spans="1:1024" ht="36" customHeight="1">
-      <c r="A67" s="15"/>
-      <c r="B67" s="16"/>
-      <c r="C67" s="16"/>
-      <c r="D67" s="16"/>
-      <c r="E67" s="17"/>
-      <c r="F67" s="33"/>
-      <c r="G67" s="33"/>
-      <c r="H67" s="34"/>
-      <c r="I67" s="20"/>
-      <c r="J67" s="21"/>
-      <c r="K67" s="21"/>
-      <c r="L67" s="21"/>
-      <c r="M67" s="21"/>
-    </row>
-    <row r="68" spans="1:1024" ht="30.75" customHeight="1">
-      <c r="B68" s="47" t="s">
-        <v>210</v>
-      </c>
-      <c r="C68" s="48"/>
-      <c r="F68" s="35"/>
-      <c r="G68" s="35"/>
-    </row>
-    <row r="69" spans="1:1024" ht="45" customHeight="1">
-      <c r="B69" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="F69" s="26"/>
-      <c r="G69" s="26"/>
-      <c r="H69" s="19">
-        <v>1</v>
-      </c>
-      <c r="I69" s="28"/>
-    </row>
-    <row r="70" spans="1:1024" ht="36" customHeight="1">
-      <c r="A70" s="15"/>
-      <c r="B70" s="16"/>
-      <c r="C70" s="16"/>
-      <c r="D70" s="16"/>
-      <c r="E70" s="17"/>
-      <c r="F70" s="49"/>
-      <c r="G70" s="49"/>
-      <c r="H70" s="50"/>
-      <c r="I70" s="51"/>
-      <c r="J70" s="21"/>
-      <c r="K70" s="21"/>
-      <c r="L70" s="21"/>
-      <c r="M70" s="21"/>
-    </row>
+    <row r="66" spans="1:1024" ht="36" customHeight="1">
+      <c r="A66" s="15"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="16"/>
+      <c r="D66" s="16"/>
+      <c r="E66" s="17"/>
+      <c r="F66" s="33"/>
+      <c r="G66" s="33"/>
+      <c r="H66" s="34"/>
+      <c r="I66" s="20"/>
+      <c r="J66" s="21"/>
+      <c r="K66" s="21"/>
+      <c r="L66" s="21"/>
+      <c r="M66" s="21"/>
+    </row>
+    <row r="67" spans="1:1024" ht="30.75" customHeight="1">
+      <c r="B67" s="47" t="s">
+        <v>192</v>
+      </c>
+      <c r="C67" s="48"/>
+      <c r="F67" s="35"/>
+      <c r="G67" s="35"/>
+    </row>
+    <row r="68" spans="1:1024" ht="77" customHeight="1">
+      <c r="B68" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="F68" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G68" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="H68" s="19"/>
+      <c r="I68" s="28"/>
+    </row>
+    <row r="69" spans="1:1024" ht="36" customHeight="1">
+      <c r="A69" s="15"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="16"/>
+      <c r="D69" s="16"/>
+      <c r="E69" s="17"/>
+      <c r="F69" s="49"/>
+      <c r="G69" s="49"/>
+      <c r="H69" s="50"/>
+      <c r="I69" s="51"/>
+      <c r="J69" s="21"/>
+      <c r="K69" s="21"/>
+      <c r="L69" s="21"/>
+      <c r="M69" s="21"/>
+    </row>
+    <row r="70" spans="1:1024" ht="14"/>
     <row r="71" spans="1:1024" ht="14"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>